<commit_message>
prepard the soter monitoring tempate
</commit_message>
<xml_diff>
--- a/data-raw/moneygram_stores.xlsx
+++ b/data-raw/moneygram_stores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcuser\OneDrive\IMPROVAST\ACS\CSIemail\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07c4d937b78de3ca/IMPROVAST/ACS/CSIemail/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97551AC-F001-48E6-BA34-B6F47A3795DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{8C708D58-5492-48AC-AD8F-B5CDC1AA76D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED68BAF8-A7DA-4687-ABE4-639A13C1DD88}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{1B6C7902-F3DE-496A-93A1-92BBFC951580}"/>
   </bookViews>
@@ -152,6 +152,12 @@
     <t>PL</t>
   </si>
   <si>
+    <t>ΧΧ</t>
+  </si>
+  <si>
+    <t>ΥΥ</t>
+  </si>
+  <si>
     <t>69361023</t>
   </si>
   <si>
@@ -216,12 +222,6 @@
   </si>
   <si>
     <t>agent_id</t>
-  </si>
-  <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>NO_MAP</t>
   </si>
 </sst>
 </file>
@@ -612,13 +612,13 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="113.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,10 +626,10 @@
         <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -640,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -651,7 +651,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,7 +662,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -695,7 +695,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -728,7 +728,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -750,7 +750,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,7 +783,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -794,7 +794,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -805,7 +805,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -816,40 +816,40 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>56</v>
+      <c r="C20" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>57</v>
+      <c r="C21" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>